<commit_message>
Added number of ensembles and traces to main ReadMe.md
</commit_message>
<xml_diff>
--- a/AnnualDifferenceInFlow/10yearsMinimumHydrologyResults.xlsx
+++ b/AnnualDifferenceInFlow/10yearsMinimumHydrologyResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Box\ColoradoRiver\LakeMeadInflow\Myers-Rosenberg\ImmersiveModelLakeMead\AnnualDifferenceInFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131153BD-BFA8-4419-8928-D3A07A953533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD55BF6-3078-4ABB-B939-E77FBAD832CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78642,7 +78642,7 @@
         <v>1259</v>
       </c>
       <c r="C6" s="4">
-        <f>$F$6-B6</f>
+        <f t="shared" ref="C6:C12" si="0">$F$6-B6</f>
         <v>1</v>
       </c>
       <c r="E6" s="4">
@@ -78663,7 +78663,7 @@
         <v>1232</v>
       </c>
       <c r="C7" s="4">
-        <f>$F$6-B7</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
@@ -78676,7 +78676,7 @@
         <v>1157</v>
       </c>
       <c r="C8" s="4">
-        <f>$F$6-B8</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
     </row>
@@ -78689,7 +78689,7 @@
         <v>928</v>
       </c>
       <c r="C9" s="4">
-        <f>$F$6-B9</f>
+        <f t="shared" si="0"/>
         <v>332</v>
       </c>
     </row>
@@ -78702,7 +78702,7 @@
         <v>640</v>
       </c>
       <c r="C10" s="4">
-        <f>$F$6-B10</f>
+        <f t="shared" si="0"/>
         <v>620</v>
       </c>
     </row>
@@ -78715,7 +78715,7 @@
         <v>373</v>
       </c>
       <c r="C11" s="4">
-        <f>$F$6-B11</f>
+        <f t="shared" si="0"/>
         <v>887</v>
       </c>
     </row>
@@ -78728,7 +78728,7 @@
         <v>150</v>
       </c>
       <c r="C12" s="4">
-        <f>$F$6-B12</f>
+        <f t="shared" si="0"/>
         <v>1110</v>
       </c>
     </row>

</xml_diff>